<commit_message>
Avisa cuantos segundos tardó el proceso por consola
</commit_message>
<xml_diff>
--- a/archivos_subir/Excel_plantilla.xlsx
+++ b/archivos_subir/Excel_plantilla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trabajo\Documents\exe-consulta\archivos_subir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B6541B-4118-413E-A6E8-B52985541643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6A9535-D312-4162-BE62-66CE9D3E7302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8742" yWindow="438" windowWidth="15360" windowHeight="9000" tabRatio="444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>FECHA DE RECEPCION</t>
   </si>
@@ -121,19 +121,7 @@
     <t>antecedentes prueba 1</t>
   </si>
   <si>
-    <t>antecedentes prueba 2</t>
-  </si>
-  <si>
-    <t>cArtá</t>
-  </si>
-  <si>
-    <t>dummy.pdf</t>
-  </si>
-  <si>
     <t>prueba materia 1</t>
-  </si>
-  <si>
-    <t>prueba materia 2</t>
   </si>
   <si>
     <t>copazo</t>
@@ -143,6 +131,12 @@
   </si>
   <si>
     <t>gbenavides</t>
+  </si>
+  <si>
+    <t>of-0009-21.pdf</t>
+  </si>
+  <si>
+    <t>Carta</t>
   </si>
 </sst>
 </file>
@@ -535,7 +529,7 @@
   <dimension ref="A1:I666"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I3"/>
+      <selection activeCell="A11" sqref="A3:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -589,55 +583,37 @@
         <v>3000</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="4">
-        <v>44829</v>
-      </c>
-      <c r="B3" s="5">
-        <v>3001</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4"/>
@@ -648,6 +624,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="6"/>
       <c r="H4" s="7"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4"/>
@@ -658,6 +635,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="6"/>
       <c r="H5" s="7"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4"/>
@@ -668,6 +646,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="6"/>
       <c r="H6" s="7"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
@@ -678,6 +657,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="6"/>
       <c r="H7" s="7"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4"/>
@@ -688,6 +668,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="6"/>
       <c r="H8" s="7"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4"/>
@@ -698,6 +679,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="6"/>
       <c r="H9" s="7"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4"/>
@@ -708,6 +690,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="6"/>
       <c r="H10" s="7"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
@@ -718,6 +701,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="6"/>
       <c r="H11" s="7"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="H12" s="2"/>

</xml_diff>

<commit_message>
Proceso comentado y limpiado
</commit_message>
<xml_diff>
--- a/archivos_subir/Excel_plantilla.xlsx
+++ b/archivos_subir/Excel_plantilla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trabajo\Documents\exe-consulta\archivos_subir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6A9535-D312-4162-BE62-66CE9D3E7302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00318E2C-1972-42C8-A0E1-A95C462FA086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8742" yWindow="438" windowWidth="15360" windowHeight="9000" tabRatio="444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="34">
   <si>
     <t>FECHA DE RECEPCION</t>
   </si>
@@ -137,6 +137,60 @@
   </si>
   <si>
     <t>Carta</t>
+  </si>
+  <si>
+    <t>prueba materia 2</t>
+  </si>
+  <si>
+    <t>antecedentes prueba 2</t>
+  </si>
+  <si>
+    <t>prueba materia 3</t>
+  </si>
+  <si>
+    <t>antecedentes prueba 3</t>
+  </si>
+  <si>
+    <t>prueba materia 4</t>
+  </si>
+  <si>
+    <t>antecedentes prueba 4</t>
+  </si>
+  <si>
+    <t>prueba materia 5</t>
+  </si>
+  <si>
+    <t>antecedentes prueba 5</t>
+  </si>
+  <si>
+    <t>prueba materia 6</t>
+  </si>
+  <si>
+    <t>antecedentes prueba 6</t>
+  </si>
+  <si>
+    <t>prueba materia 7</t>
+  </si>
+  <si>
+    <t>antecedentes prueba 7</t>
+  </si>
+  <si>
+    <t>prueba materia 8</t>
+  </si>
+  <si>
+    <t>antecedentes prueba 8</t>
+  </si>
+  <si>
+    <t>prueba materia 9</t>
+  </si>
+  <si>
+    <t>antecedentes prueba 9</t>
+  </si>
+  <si>
+    <t>prueba materia 10</t>
+  </si>
+  <si>
+    <t>antecedentes prueba 10</t>
   </si>
 </sst>
 </file>
@@ -529,7 +583,7 @@
   <dimension ref="A1:I666"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A3:I11"/>
+      <selection activeCell="I2" sqref="A2:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -605,103 +659,265 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="6"/>
+      <c r="A3" s="4">
+        <v>44829</v>
+      </c>
+      <c r="B3" s="5">
+        <v>3001</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="6"/>
+      <c r="A4" s="4">
+        <v>44830</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3002</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="6"/>
+      <c r="A5" s="4">
+        <v>44831</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3003</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="6"/>
+      <c r="A6" s="4">
+        <v>44832</v>
+      </c>
+      <c r="B6" s="5">
+        <v>3004</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="6"/>
+      <c r="A7" s="4">
+        <v>44833</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3005</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="6"/>
+      <c r="A8" s="4">
+        <v>44834</v>
+      </c>
+      <c r="B8" s="5">
+        <v>3006</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="6"/>
+      <c r="A9" s="4">
+        <v>44835</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3007</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="6"/>
+      <c r="A10" s="4">
+        <v>44836</v>
+      </c>
+      <c r="B10" s="5">
+        <v>3008</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="6"/>
+      <c r="A11" s="4">
+        <v>44837</v>
+      </c>
+      <c r="B11" s="5">
+        <v>3009</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="H12" s="2"/>

</xml_diff>